<commit_message>
add psy course analysis
</commit_message>
<xml_diff>
--- a/api/python/TaiGerTranscriptAnalyzerJS/database/Psychology/PSY_Programs.xlsx
+++ b/api/python/TaiGerTranscriptAnalyzerJS/database/Psychology/PSY_Programs.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjMYeE+Pf3Aio1fElLigekXuO0cEg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj8nsEue5EPrJkwE+1bTgyBc65DWg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Program</t>
   </si>
@@ -30,12 +30,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>LMU_NEURO_COGN_PSYCHOLOGY</t>
-  </si>
-  <si>
-    <t>FU_BERLIN_COGN_NEUROSCIENCE</t>
-  </si>
-  <si>
     <t>TU_BERLIN_COMP_NEUROSCIENCE</t>
   </si>
   <si>
@@ -46,6 +40,9 @@
   </si>
   <si>
     <t>UNI_OLDENBURG_NEUROCOGN_PSY</t>
+  </si>
+  <si>
+    <t>TU_DARMSTADT_COGNITIVE_SCIENCE</t>
   </si>
 </sst>
 </file>
@@ -363,14 +360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="8" ht="14.25" customHeight="1"/>
     <row r="9" ht="14.25" customHeight="1"/>
     <row r="10" ht="14.25" customHeight="1"/>
     <row r="11" ht="14.25" customHeight="1"/>
@@ -1361,11 +1351,9 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B1:B8">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B1:B7">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>